<commit_message>
worked on somthing that is not good
</commit_message>
<xml_diff>
--- a/admin.xlsx
+++ b/admin.xlsx
@@ -175,12 +175,12 @@
   <dimension ref="A1:C86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26"/>
   </cols>
@@ -206,7 +206,7 @@
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
         <v>20333510</v>
       </c>
@@ -537,8 +537,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>